<commit_message>
adds trap start and end to recapture metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_recapture_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_recapture_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3343A0-2A2F-4E33-A831-C4AA432436BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E14DA4-5499-4216-8FCC-EC5196C146A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="1060" windowWidth="19900" windowHeight="13150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="2390" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -213,6 +213,27 @@
   <si>
     <t>position of mark on body of fish. Level = "Whole body", "Nose"</t>
   </si>
+  <si>
+    <t>trap_start_date</t>
+  </si>
+  <si>
+    <t>Start date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t>trap_end_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> End date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t>2024-03-29 10:45:51</t>
+  </si>
+  <si>
+    <t>2022-02-02 10:00:10</t>
+  </si>
+  <si>
+    <t>2024-03-31 08:30:21</t>
+  </si>
 </sst>
 </file>
 
@@ -280,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -307,6 +328,9 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,8 +549,8 @@
   <dimension ref="A1:Z982"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1269,19 +1293,35 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
+      <c r="J19" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="L19" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1297,19 +1337,35 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
+      <c r="J20" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="L20" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -28261,8 +28317,7 @@
       <c r="Z982" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A19:A20"/>
+  <mergeCells count="1">
     <mergeCell ref="A21:A22"/>
   </mergeCells>
   <dataValidations count="4">

</xml_diff>